<commit_message>
New Branch for work
</commit_message>
<xml_diff>
--- a/ScumSprint/Stories.xlsx
+++ b/ScumSprint/Stories.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Story1</t>
   </si>
@@ -130,6 +130,24 @@
   </si>
   <si>
     <t>Write code for he vision of the password edit text</t>
+  </si>
+  <si>
+    <t>pushing to master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">completing the first version </t>
+  </si>
+  <si>
+    <t>make Shopkeeper project</t>
+  </si>
+  <si>
+    <t>Testing github push and fetch</t>
+  </si>
+  <si>
+    <t>desing shopkeeper form</t>
+  </si>
+  <si>
+    <t>write code for applications buttons</t>
   </si>
 </sst>
 </file>
@@ -139,7 +157,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-408]General"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +172,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="161"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="161"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -228,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -246,6 +272,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -812,7 +839,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I16" sqref="I16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,7 +959,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="15"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -967,10 +994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,8 +1081,11 @@
       <c r="D3" s="14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1064,6 +1094,9 @@
       </c>
       <c r="D4" s="14" t="s">
         <v>31</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -1076,6 +1109,9 @@
       <c r="D5" s="14" t="s">
         <v>32</v>
       </c>
+      <c r="G5" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1087,6 +1123,9 @@
       <c r="D6" s="14" t="s">
         <v>33</v>
       </c>
+      <c r="G6" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1097,6 +1136,14 @@
       </c>
       <c r="D7" s="14" t="s">
         <v>34</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
program ready for lunch
1.2
</commit_message>
<xml_diff>
--- a/ScumSprint/Stories.xlsx
+++ b/ScumSprint/Stories.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Project2017\ScumSprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Vagrad/Documents/GitHub/Project2017/ScumSprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Story1</t>
   </si>
@@ -130,6 +136,36 @@
   </si>
   <si>
     <t>Write code for he vision of the password edit text</t>
+  </si>
+  <si>
+    <t>Testing github push and fech</t>
+  </si>
+  <si>
+    <t>make Shopkeeper project</t>
+  </si>
+  <si>
+    <t>desine shopkeeper form</t>
+  </si>
+  <si>
+    <t>whrite code for applications buttons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">completing the first version </t>
+  </si>
+  <si>
+    <t>pushing to master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">importing new setting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">whrite the code to merge the programs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">merge complete </t>
+  </si>
+  <si>
+    <t xml:space="preserve">learn on youtube how to merge layout in androin studio </t>
   </si>
 </sst>
 </file>
@@ -156,7 +192,7 @@
       <charset val="161"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +235,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -228,7 +270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -244,6 +286,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -592,9 +638,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -627,9 +673,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -811,19 +857,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="10" width="11" customWidth="1"/>
     <col min="11" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -859,7 +905,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -875,7 +921,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -891,7 +937,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
@@ -907,7 +953,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -923,15 +969,15 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -939,7 +985,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>16</v>
       </c>
@@ -955,7 +1001,7 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:12" ht="16" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -967,23 +1013,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1021,7 +1067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1044,7 +1090,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1054,8 +1100,11 @@
       <c r="D3" s="14" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1065,8 +1114,11 @@
       <c r="D4" s="14" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="G4" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1076,8 +1128,11 @@
       <c r="D5" s="14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="G5" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1087,8 +1142,11 @@
       <c r="D6" s="14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="G6" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1097,6 +1155,34 @@
       </c>
       <c r="D7" s="14" t="s">
         <v>34</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G8" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="60" x14ac:dyDescent="0.2">
+      <c r="G9" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="G10" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="G11" s="16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="G12" s="16" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>